<commit_message>
New ADS Drawing Pictures
Also filled in my weekly availability for this semester
</commit_message>
<xml_diff>
--- a/weekly availability.xlsx
+++ b/weekly availability.xlsx
@@ -94,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -173,9 +179,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +492,7 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,24 +632,24 @@
       </c>
     </row>
     <row r="3" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
       <c r="AH3" s="9"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
@@ -806,7 +815,7 @@
       </c>
     </row>
     <row r="8" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -822,20 +831,20 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="5"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
@@ -1008,22 +1017,31 @@
       </c>
     </row>
     <row r="13" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16"/>
       <c r="AH13" s="10"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -1185,15 +1203,26 @@
       </c>
     </row>
     <row r="18" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16"/>
       <c r="AH18" s="10"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
@@ -1359,22 +1388,33 @@
       </c>
     </row>
     <row r="23" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
       <c r="AH23" s="10"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -1536,16 +1576,20 @@
       </c>
     </row>
     <row r="28" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="14"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
       <c r="AH28" s="10"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
@@ -1703,12 +1747,24 @@
       </c>
     </row>
     <row r="33" spans="1:34" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
       <c r="AH33" s="10"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
@@ -1869,6 +1925,7 @@
         <v>14</v>
       </c>
       <c r="G40" s="2"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="E42" t="s">

</xml_diff>